<commit_message>
added docker references and commands
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj_Thodupunuri\Desktop\Dheeraj\Notes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Angular JS" sheetId="1" r:id="rId1"/>
@@ -20,13 +15,14 @@
     <sheet name="References" sheetId="4" r:id="rId6"/>
     <sheet name="npm commands" sheetId="5" r:id="rId7"/>
     <sheet name="Learnings" sheetId="9" r:id="rId8"/>
+    <sheet name="Docker " sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Learnings!$A$1:$D$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="147">
   <si>
     <t>Topic</t>
   </si>
@@ -395,12 +391,105 @@
   <si>
     <t>Repository pattern</t>
   </si>
+  <si>
+    <t xml:space="preserve">docker images </t>
+  </si>
+  <si>
+    <t>Lists down all docker images</t>
+  </si>
+  <si>
+    <t>docker ps</t>
+  </si>
+  <si>
+    <t>Lists down all docker images in format</t>
+  </si>
+  <si>
+    <t>Lists down all running images(without any format - squished)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker ps -a </t>
+  </si>
+  <si>
+    <t>Lists down all containers (including stopped containers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker ps -l </t>
+  </si>
+  <si>
+    <t>Lists down the last container</t>
+  </si>
+  <si>
+    <t>docker ps --format= $FORMAT</t>
+  </si>
+  <si>
+    <t>docker  commit  "container ID"</t>
+  </si>
+  <si>
+    <t>To create new image from container</t>
+  </si>
+  <si>
+    <t>docker tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker version </t>
+  </si>
+  <si>
+    <t>displays the version of docker</t>
+  </si>
+  <si>
+    <t>docker stop "container-name"</t>
+  </si>
+  <si>
+    <t>stops the container</t>
+  </si>
+  <si>
+    <t>docker rm "containerID"</t>
+  </si>
+  <si>
+    <t>Deletes or removes the container</t>
+  </si>
+  <si>
+    <t>docker image rm "Image ID"</t>
+  </si>
+  <si>
+    <t>To remove the docker image.</t>
+  </si>
+  <si>
+    <t>docker pull "imge"</t>
+  </si>
+  <si>
+    <t>Just downloads the images , but does not starts the container.</t>
+  </si>
+  <si>
+    <t>docker run -it</t>
+  </si>
+  <si>
+    <t>To run image and make container in interactive mode</t>
+  </si>
+  <si>
+    <t>docker run -d</t>
+  </si>
+  <si>
+    <t>To run comtainer in detached mode</t>
+  </si>
+  <si>
+    <t>docker start "container-name"</t>
+  </si>
+  <si>
+    <t>To restart the container.</t>
+  </si>
+  <si>
+    <t>https://medium.com/codingthesmartway-com-blog/docker-beginners-guide-part-1-images-containers-6f3507fffc98</t>
+  </si>
+  <si>
+    <t>Docker Image and Containers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +565,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -490,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -534,6 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,7 +691,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -630,7 +726,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -807,27 +903,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="93.140625" customWidth="1"/>
     <col min="2" max="2" width="89.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -838,7 +934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -846,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -854,7 +950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -869,14 +965,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="87" bestFit="1" customWidth="1"/>
@@ -885,7 +981,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
@@ -902,7 +998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -913,7 +1009,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -924,7 +1020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -935,7 +1031,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -946,7 +1042,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -957,7 +1053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -968,7 +1064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="18" t="s">
         <v>84</v>
       </c>
@@ -982,7 +1078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="17" t="s">
@@ -992,7 +1088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="17" t="s">
@@ -1002,7 +1098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1016,7 +1112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>93</v>
       </c>
@@ -1024,7 +1120,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -1035,7 +1131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -1049,7 +1145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1080,20 +1176,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1101,7 +1197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1124,20 +1220,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="72" customWidth="1"/>
     <col min="2" max="2" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1159,20 +1255,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
@@ -1180,7 +1276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1188,7 +1284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1204,7 +1300,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1212,7 +1308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1226,21 +1322,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="100.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1262,7 +1358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -1273,7 +1369,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
@@ -1284,21 +1380,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -1309,7 +1405,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>109</v>
       </c>
@@ -1320,7 +1416,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>114</v>
       </c>
@@ -1329,6 +1425,17 @@
       </c>
       <c r="C9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1345,27 +1452,28 @@
     <hyperlink ref="A6" r:id="rId6"/>
     <hyperlink ref="A8" r:id="rId7"/>
     <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="127.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1379,7 +1487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1404,7 +1512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="19" t="s">
         <v>34</v>
       </c>
@@ -1415,12 +1523,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="19"/>
       <c r="B5" s="20"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="19"/>
       <c r="B6" s="20"/>
       <c r="D6" s="18"/>
@@ -1440,15 +1548,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1456,7 +1564,7 @@
     <col min="4" max="4" width="98.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1481,7 +1589,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1492,7 +1600,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1503,7 +1611,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1514,7 +1622,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1528,7 +1636,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1539,7 +1647,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1550,7 +1658,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1561,7 +1669,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1572,7 +1680,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1583,7 +1691,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1597,7 +1705,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1611,7 +1719,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="16" t="s">
         <v>76</v>
       </c>
@@ -1622,7 +1730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1">
       <c r="A15" s="18" t="s">
         <v>91</v>
       </c>
@@ -1636,7 +1744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1644,7 +1752,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1655,7 +1763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -1663,7 +1771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1677,7 +1785,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1">
       <c r="A20" s="18" t="s">
         <v>106</v>
       </c>
@@ -1691,12 +1799,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -1738,4 +1846,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added few references to
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj_Thodupunuri\Desktop\Dheeraj\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj_Thodupunuri\Desktop\Dheeraj\Drj\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Angular JS" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Learnings!$A$1:$D$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
   <si>
     <t>Topic</t>
   </si>
@@ -394,6 +395,24 @@
   </si>
   <si>
     <t>Repository pattern</t>
+  </si>
+  <si>
+    <t>ng test</t>
+  </si>
+  <si>
+    <t>runs test cases and opens report in browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity framework core </t>
+  </si>
+  <si>
+    <t>https://www.tektutorialshub.com/linq-to-entities/linq-to-entities-tutorial/</t>
+  </si>
+  <si>
+    <t>Linq To Entities</t>
+  </si>
+  <si>
+    <t>Entity Framework Core</t>
   </si>
 </sst>
 </file>
@@ -870,10 +889,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +955,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1063,7 +1083,22 @@
         <v>49</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E15">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
@@ -1160,16 +1195,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,6 +1253,14 @@
       </c>
       <c r="B6" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1227,17 +1270,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="100.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1329,6 +1372,17 @@
       </c>
       <c r="C9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1345,6 +1399,7 @@
     <hyperlink ref="A6" r:id="rId6"/>
     <hyperlink ref="A8" r:id="rId7"/>
     <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed file extension to .txt
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj_Thodupunuri\Desktop\Dheeraj\Drj\Notes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Angular JS" sheetId="1" r:id="rId1"/>
@@ -20,14 +15,15 @@
     <sheet name="References" sheetId="4" r:id="rId6"/>
     <sheet name="npm commands" sheetId="5" r:id="rId7"/>
     <sheet name="Learnings" sheetId="9" r:id="rId8"/>
+    <sheet name="Docker" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Learnings!$A$1:$D$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
   <si>
     <t>Topic</t>
   </si>
@@ -414,12 +410,30 @@
   <si>
     <t>Entity Framework Core</t>
   </si>
+  <si>
+    <t>docker logs "container-name"</t>
+  </si>
+  <si>
+    <t>logs all messages related to that container</t>
+  </si>
+  <si>
+    <t>docker kill "container-name"</t>
+  </si>
+  <si>
+    <t>Stops the container - stopped container</t>
+  </si>
+  <si>
+    <t>docker rm "container-name"</t>
+  </si>
+  <si>
+    <t>Removes / Deletes the container</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -649,7 +663,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -826,27 +840,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="93.140625" customWidth="1"/>
     <col min="2" max="2" width="89.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -857,7 +871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -865,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -873,7 +887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -888,7 +902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -896,7 +910,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="87" bestFit="1" customWidth="1"/>
@@ -905,7 +919,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
@@ -922,7 +936,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -933,7 +947,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -944,7 +958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -955,7 +969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -966,7 +980,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -977,7 +991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="18" t="s">
         <v>84</v>
       </c>
@@ -1002,7 +1016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="17" t="s">
@@ -1012,7 +1026,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="17" t="s">
@@ -1022,7 +1036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1036,7 +1050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>93</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -1055,7 +1069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -1069,7 +1083,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1083,7 +1097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1115,20 +1129,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1159,20 +1173,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="72" customWidth="1"/>
     <col min="2" max="2" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1194,20 +1208,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1223,7 +1237,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1239,7 +1253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1247,7 +1261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1255,7 +1269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -1269,21 +1283,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="100.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1305,7 +1319,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -1316,7 +1330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
@@ -1327,21 +1341,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -1352,7 +1366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>109</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>114</v>
       </c>
@@ -1374,7 +1388,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>119</v>
       </c>
@@ -1406,21 +1420,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="127.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1434,7 +1448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1459,7 +1473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="19" t="s">
         <v>34</v>
       </c>
@@ -1470,12 +1484,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="19"/>
       <c r="B5" s="20"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="19"/>
       <c r="B6" s="20"/>
       <c r="D6" s="18"/>
@@ -1495,15 +1509,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1511,7 +1525,7 @@
     <col min="4" max="4" width="98.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1539,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1536,7 +1550,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1547,7 +1561,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1569,7 +1583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1583,7 +1597,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1594,7 +1608,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1605,7 +1619,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1616,7 +1630,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1627,7 +1641,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1638,7 +1652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1652,7 +1666,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1666,7 +1680,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="16" t="s">
         <v>76</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1">
       <c r="A15" s="18" t="s">
         <v>91</v>
       </c>
@@ -1691,7 +1705,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1699,7 +1713,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1710,7 +1724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -1718,7 +1732,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1732,7 +1746,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1">
       <c r="A20" s="18" t="s">
         <v>106</v>
       </c>
@@ -1746,12 +1760,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -1793,4 +1807,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added windows commands workbook
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -16,6 +16,7 @@
     <sheet name="npm commands" sheetId="5" r:id="rId7"/>
     <sheet name="Learnings" sheetId="9" r:id="rId8"/>
     <sheet name="Docker" sheetId="10" r:id="rId9"/>
+    <sheet name="Windows Commands" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Learnings!$A$1:$D$22</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
   <si>
     <t>Topic</t>
   </si>
@@ -428,12 +429,120 @@
   <si>
     <t>Removes / Deletes the container</t>
   </si>
+  <si>
+    <t xml:space="preserve">docker images </t>
+  </si>
+  <si>
+    <t>lists all downloaded images</t>
+  </si>
+  <si>
+    <t>To look at recently stopped container</t>
+  </si>
+  <si>
+    <t>docker ps -l --format=$Format</t>
+  </si>
+  <si>
+    <t>docker commit "container-ID" "give image name"</t>
+  </si>
+  <si>
+    <t>To name an image</t>
+  </si>
+  <si>
+    <t>docker commit "container-ID" "give image name":"version"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Names an image with the tag which you have specified as version in command </t>
+  </si>
+  <si>
+    <t>docker pull "image-name"</t>
+  </si>
+  <si>
+    <t>Pulls an image from registry , by default it pulls from "Docker-Hub"</t>
+  </si>
+  <si>
+    <t>docker rmi image-name:tag</t>
+  </si>
+  <si>
+    <t>Removes an image with the specified tag</t>
+  </si>
+  <si>
+    <t>docker rmii image-id</t>
+  </si>
+  <si>
+    <t>Removes an image with the specified image id</t>
+  </si>
+  <si>
+    <t>cls</t>
+  </si>
+  <si>
+    <t>Clears the screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dir </t>
+  </si>
+  <si>
+    <t>Lists all the directories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates a directory with the specified name </t>
+  </si>
+  <si>
+    <t>mkdir</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>Will print the current working directory</t>
+  </si>
+  <si>
+    <t>dir/s</t>
+  </si>
+  <si>
+    <t>Lists the files in the current working directory</t>
+  </si>
+  <si>
+    <t>docker run -ti -v C:\Users\pcs\example:/shared-folder ubuntu bash</t>
+  </si>
+  <si>
+    <t>Shares data between host and container</t>
+  </si>
+  <si>
+    <t>docker run -ti -v /shared-data ubuntu bash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates a volume(shared-data) </t>
+  </si>
+  <si>
+    <t>docker run -ti --volumes-from nostalgic_wescoff ubuntu bash</t>
+  </si>
+  <si>
+    <t>Shares data from the container specified(nostalgic_wescoff) into its container</t>
+  </si>
+  <si>
+    <t>docker search "image-name"</t>
+  </si>
+  <si>
+    <t>Searches the specified image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker ps -a </t>
+  </si>
+  <si>
+    <t>To list down all stopped and running containers</t>
+  </si>
+  <si>
+    <t>docker run "image-name"</t>
+  </si>
+  <si>
+    <t>Runs an image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,8 +586,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +624,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -523,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -567,6 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -840,7 +962,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -898,6 +1020,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1811,16 +2001,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1847,6 +2037,110 @@
         <v>127</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added few references to docker workbook
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Angular JS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="177">
   <si>
     <t>Topic</t>
   </si>
@@ -537,12 +537,51 @@
   <si>
     <t>Runs an image</t>
   </si>
+  <si>
+    <t>docker inspect "container-ID"</t>
+  </si>
+  <si>
+    <t>Provides more detailed information about container</t>
+  </si>
+  <si>
+    <t>docker logs "container-ID"</t>
+  </si>
+  <si>
+    <t>Will display messages the container has written to standard error or standard out.</t>
+  </si>
+  <si>
+    <t>docker inspect '{{.State.Pid}}' "Container-name"</t>
+  </si>
+  <si>
+    <t>docker run -d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runs the container in detached mode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker run -d -p 5000:5000 --restart = always </t>
+  </si>
+  <si>
+    <t>restarts option says to restart the container , when ever container shuts down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker save -o my-images.tar.gz "images with space seperated" </t>
+  </si>
+  <si>
+    <t>This docker command saves the specified images to the specified folder(my-inage.tar.gz).Option -O is output.</t>
+  </si>
+  <si>
+    <t>docker load -I my-images.tar.gz</t>
+  </si>
+  <si>
+    <t>Option -I is Input.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +630,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -644,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,6 +724,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,7 +735,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1038,10 +1084,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1193,10 +1239,10 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -1207,8 +1253,8 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="17" t="s">
         <v>88</v>
       </c>
@@ -1217,8 +1263,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="17" t="s">
         <v>89</v>
       </c>
@@ -1524,10 +1570,10 @@
       <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1535,15 +1581,15 @@
       <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
@@ -1664,25 +1710,25 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="D5" s="18"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="D6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1882,13 +1928,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" hidden="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1896,9 +1942,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" hidden="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
         <v>101</v>
       </c>
@@ -1937,13 +1983,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" hidden="1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1951,9 +1997,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" hidden="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:4" hidden="1">
       <c r="A22" t="s">
@@ -2001,16 +2047,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2141,7 +2187,61 @@
         <v>163</v>
       </c>
     </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
+      <c r="A18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added few refernces to excel sheet and info  to docker.txt
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Angular JS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Learnings!$A$1:$D$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="181">
   <si>
     <t>Topic</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>hyphen t option is used to tag an image to a specified name</t>
+  </si>
+  <si>
+    <t>https://www.learnitguide.net/2018/06/docker-onbuild-command-with-examples.html</t>
+  </si>
+  <si>
+    <t>ONBUILD Docker instruction</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1155,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,7 +1250,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" s="20" t="s">
         <v>84</v>
       </c>
@@ -1254,29 +1260,25 @@
       <c r="C8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" hidden="1">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1339,7 +1341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" hidden="1">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1348,16 +1350,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E15">
+  <autoFilter ref="A1:E16">
     <filterColumn colId="4">
       <filters>
         <filter val="Open"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
@@ -1526,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,6 +1642,17 @@
       </c>
       <c r="C10" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1656,6 +1670,7 @@
     <hyperlink ref="A8" r:id="rId7"/>
     <hyperlink ref="A9" r:id="rId8"/>
     <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2055,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>